<commit_message>
minor changes and fixed an interface bug
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HybridRocket\PurdueHybridRocket2018-19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79AEC4D8-EFD5-4F0C-9835-9B0EF7D8A546}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B255015B-4BC3-4B18-82A4-19D5AEAD6E0C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9735" xr2:uid="{ACBDC250-2DBD-45AA-9159-328A8853C6A6}"/>
   </bookViews>
@@ -411,7 +411,7 @@
   <dimension ref="A10:J2170"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11:J2170"/>
+      <selection activeCell="A10" sqref="A10:J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>